<commit_message>
fixed getRefreshToken() doesn't need to update info after ReAuthentication
</commit_message>
<xml_diff>
--- a/app_cache/verykship_shipment.xlsx
+++ b/app_cache/verykship_shipment.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AJ3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD4"/>
@@ -660,6 +660,262 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Audrey Xu</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>7783179726</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>3302-4670 Assembly Way</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Burnaby</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>BC</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>V5H 0H3</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Lakeasha Tyson</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>7788386913</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>1106 N Driver st</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>DURHAM</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>27701</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Pak</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>"Gold Filled Beads"</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>55.00</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>180</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Audrey Xu</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>7783179726</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>3302-4670 Assembly Way</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Burnaby</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>BC</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>V5H 0H3</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Cynthia Dekker</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>7788386913</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>370 Silverwood Ave</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Welland</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>L3C 0C6</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Pak</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>"Gold Filled Beads"</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>256.50</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>